<commit_message>
Dodanie zasilenia podstawowych statystyk dotyczących lotu oraz powiązanej z nim linią lotniczą i lotniskami
</commit_message>
<xml_diff>
--- a/ssis_hd/sql/facts_mapping.xlsx
+++ b/ssis_hd/sql/facts_mapping.xlsx
@@ -189,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -198,9 +198,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -210,25 +208,193 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -236,6 +402,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:B44" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:B44"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Kolumna" dataDxfId="2"/>
+    <tableColumn id="2" name="Nr mapowania" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,21 +704,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A44"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -549,7 +726,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>0</v>
       </c>
     </row>
@@ -557,7 +734,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
     </row>
@@ -565,7 +742,7 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
     </row>
@@ -573,7 +750,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
     </row>
@@ -581,7 +758,7 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>4</v>
       </c>
     </row>
@@ -589,7 +766,7 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>5</v>
       </c>
     </row>
@@ -597,7 +774,7 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>6</v>
       </c>
     </row>
@@ -605,7 +782,7 @@
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>7</v>
       </c>
     </row>
@@ -613,7 +790,7 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>8</v>
       </c>
     </row>
@@ -621,7 +798,7 @@
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>9</v>
       </c>
     </row>
@@ -629,7 +806,7 @@
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>10</v>
       </c>
     </row>
@@ -637,7 +814,7 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>11</v>
       </c>
     </row>
@@ -645,7 +822,7 @@
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>12</v>
       </c>
     </row>
@@ -653,7 +830,7 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>13</v>
       </c>
     </row>
@@ -661,7 +838,7 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>14</v>
       </c>
     </row>
@@ -669,7 +846,7 @@
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>15</v>
       </c>
     </row>
@@ -677,7 +854,7 @@
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>16</v>
       </c>
     </row>
@@ -685,7 +862,7 @@
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>17</v>
       </c>
     </row>
@@ -693,7 +870,7 @@
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>18</v>
       </c>
     </row>
@@ -701,7 +878,7 @@
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>19</v>
       </c>
     </row>
@@ -709,7 +886,7 @@
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>20</v>
       </c>
     </row>
@@ -717,7 +894,7 @@
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>21</v>
       </c>
     </row>
@@ -725,7 +902,7 @@
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>22</v>
       </c>
     </row>
@@ -733,7 +910,7 @@
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>23</v>
       </c>
     </row>
@@ -741,7 +918,7 @@
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>24</v>
       </c>
     </row>
@@ -749,7 +926,7 @@
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>25</v>
       </c>
     </row>
@@ -757,7 +934,7 @@
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>26</v>
       </c>
     </row>
@@ -765,7 +942,7 @@
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>27</v>
       </c>
     </row>
@@ -773,7 +950,7 @@
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>28</v>
       </c>
     </row>
@@ -781,7 +958,7 @@
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>29</v>
       </c>
     </row>
@@ -789,7 +966,7 @@
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>30</v>
       </c>
     </row>
@@ -797,7 +974,7 @@
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>31</v>
       </c>
     </row>
@@ -805,7 +982,7 @@
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>32</v>
       </c>
     </row>
@@ -813,7 +990,7 @@
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>33</v>
       </c>
     </row>
@@ -821,7 +998,7 @@
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>34</v>
       </c>
     </row>
@@ -829,7 +1006,7 @@
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>35</v>
       </c>
     </row>
@@ -837,7 +1014,7 @@
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>36</v>
       </c>
     </row>
@@ -845,7 +1022,7 @@
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>37</v>
       </c>
     </row>
@@ -853,7 +1030,7 @@
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>38</v>
       </c>
     </row>
@@ -861,7 +1038,7 @@
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
         <v>39</v>
       </c>
     </row>
@@ -869,7 +1046,7 @@
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="2">
         <v>40</v>
       </c>
     </row>
@@ -877,21 +1054,24 @@
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="6">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Zmiana pakietu zasilającego tabelę faktów
</commit_message>
<xml_diff>
--- a/ssis_hd/sql/facts_mapping.xlsx
+++ b/ssis_hd/sql/facts_mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Kolumna</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>LateAircraftDelay</t>
+  </si>
+  <si>
+    <t>ArrDelayGroup</t>
   </si>
 </sst>
 </file>
@@ -297,6 +300,70 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -330,70 +397,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -405,11 +408,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:B44" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:B44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:B45" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="A1:B45"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Kolumna" dataDxfId="2"/>
-    <tableColumn id="2" name="Nr mapowania" dataDxfId="1"/>
+    <tableColumn id="1" name="Kolumna" dataDxfId="1"/>
+    <tableColumn id="2" name="Nr mapowania" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -702,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,6 +1067,14 @@
       </c>
       <c r="B44" s="6">
         <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="6">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Poprawa pakietu ładującego dane do tabeli faktów
</commit_message>
<xml_diff>
--- a/ssis_hd/sql/facts_mapping.xlsx
+++ b/ssis_hd/sql/facts_mapping.xlsx
@@ -27,9 +27,6 @@
     <t>LocalScheduledDepartureTime</t>
   </si>
   <si>
-    <t>DelayGroup</t>
-  </si>
-  <si>
     <t>DifficultiesKey</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>ArrDelayGroup</t>
+  </si>
+  <si>
+    <t>DepDelayGroup</t>
   </si>
 </sst>
 </file>
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +735,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
         <v>7</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
         <v>8</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
         <v>9</v>
@@ -807,7 +807,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
         <v>10</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2">
         <v>11</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
         <v>12</v>
@@ -831,7 +831,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2">
         <v>13</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2">
         <v>14</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2">
         <v>15</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2">
         <v>16</v>
@@ -863,7 +863,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2">
         <v>17</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2">
         <v>18</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2">
         <v>19</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>20</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2">
         <v>21</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2">
         <v>22</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2">
         <v>23</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2">
         <v>24</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2">
         <v>25</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2">
         <v>26</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2">
         <v>27</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2">
         <v>28</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2">
         <v>29</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="2">
         <v>30</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2">
         <v>31</v>
@@ -983,7 +983,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2">
         <v>32</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="2">
         <v>33</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="2">
         <v>34</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="2">
         <v>35</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="2">
         <v>36</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="2">
         <v>37</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2">
         <v>38</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2">
         <v>39</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2">
         <v>40</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="2">
         <v>41</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="6">
         <v>42</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="6">
         <v>43</v>

</xml_diff>